<commit_message>
Added constant distribution with no value to each user input
</commit_message>
<xml_diff>
--- a/InputFiles/User Inputs.xlsx
+++ b/InputFiles/User Inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7718B18B-E17D-46C6-AD86-90E84B439799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEAED39-0BEE-4A47-B506-5CB2404EA9B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1176" yWindow="1224" windowWidth="17280" windowHeight="9060" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="76">
   <si>
     <t>SCWAD</t>
   </si>
@@ -2406,7 +2406,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2692,7 +2692,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2755,7 +2755,9 @@
       <c r="E2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -2775,7 +2777,9 @@
       <c r="E3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="14" t="s">
+        <v>3</v>
+      </c>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -2808,8 +2812,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2872,7 +2876,9 @@
       <c r="E2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -2892,7 +2898,9 @@
       <c r="E3" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
@@ -2912,7 +2920,9 @@
       <c r="E4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
@@ -2947,7 +2957,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3010,7 +3020,9 @@
       <c r="E2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -3030,7 +3042,9 @@
       <c r="E3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
@@ -3050,7 +3064,9 @@
       <c r="E4" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
@@ -3090,7 +3106,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3153,7 +3169,9 @@
       <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -3173,7 +3191,9 @@
       <c r="E3" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
@@ -3193,7 +3213,9 @@
       <c r="E4" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
@@ -3213,7 +3235,9 @@
       <c r="E5" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="11"/>
+      <c r="F5" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
@@ -3233,7 +3257,9 @@
       <c r="E6" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -3260,7 +3286,7 @@
       <formula>ISBLANK($F6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
@@ -3366,8 +3392,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3430,7 +3456,9 @@
       <c r="E2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>

</xml_diff>

<commit_message>
Get controllers and services hooked up to provide client input file information.
</commit_message>
<xml_diff>
--- a/InputFiles/User Inputs.xlsx
+++ b/InputFiles/User Inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\EPA\WideAreaDecon\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEAED39-0BEE-4A47-B506-5CB2404EA9B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2AEC35-D3B3-458A-A0D4-D3C7B2187028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1176" yWindow="1224" windowWidth="17280" windowHeight="9060" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -2410,9 +2410,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2434,14 +2434,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2550,34 +2550,34 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <f>ROWS($A$10:A10)</f>
         <v>1</v>
@@ -2586,7 +2586,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <f>ROWS($A$10:A11)</f>
         <v>2</v>
@@ -2595,7 +2595,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <f>ROWS($A$10:A12)</f>
         <v>3</v>
@@ -2604,7 +2604,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <f>ROWS($A$10:A13)</f>
         <v>4</v>
@@ -2613,7 +2613,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <f>ROWS($A$10:A14)</f>
         <v>5</v>
@@ -2622,7 +2622,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>6</v>
       </c>
@@ -2630,12 +2630,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2643,17 +2643,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2661,22 +2661,22 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E29" t="s">
         <v>32</v>
       </c>
@@ -2691,25 +2691,25 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.26953125" customWidth="1"/>
+    <col min="5" max="5" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>42</v>
@@ -2763,7 +2763,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="13" t="s">
         <v>43</v>
@@ -2816,21 +2816,21 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.7265625" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>43</v>
@@ -2884,7 +2884,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>52</v>
@@ -2906,7 +2906,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>43</v>
@@ -2960,21 +2960,21 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.26953125" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>42</v>
@@ -3028,7 +3028,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>57</v>
@@ -3050,7 +3050,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>52</v>
@@ -3109,21 +3109,21 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.1796875" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>42</v>
@@ -3177,7 +3177,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="11" t="s">
         <v>43</v>
@@ -3199,7 +3199,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
         <v>43</v>
@@ -3221,7 +3221,7 @@
       <c r="I4" s="11"/>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
         <v>43</v>
@@ -3243,7 +3243,7 @@
       <c r="I5" s="11"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
         <v>52</v>
@@ -3306,21 +3306,21 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3392,25 +3392,25 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.81640625" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Add in min / max logistic values to all parameters
</commit_message>
<xml_diff>
--- a/InputFiles/User Inputs.xlsx
+++ b/InputFiles/User Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\EPA\WideAreaDecon\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2AEC35-D3B3-458A-A0D4-D3C7B2187028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE0009D-57EE-4206-84A5-AAA4F38DF551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="79">
   <si>
     <t>SCWAD</t>
   </si>
@@ -270,6 +270,15 @@
   </si>
   <si>
     <t>Price per roundrtip ticket per person</t>
+  </si>
+  <si>
+    <t>Lower Limit</t>
+  </si>
+  <si>
+    <t>Upper Limit</t>
+  </si>
+  <si>
+    <t>Step</t>
   </si>
 </sst>
 </file>
@@ -305,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -485,12 +494,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -507,12 +527,391 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="102">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -1990,117 +2389,135 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table156" displayName="Table156" ref="A1:J3" totalsRowShown="0" tableBorderDxfId="81">
-  <autoFilter ref="A1:J3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Internal" dataDxfId="80"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="78"/>
-    <tableColumn id="10" xr3:uid="{115A314C-6A1B-4509-AD17-EBA48B227F1D}" name="Description" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Units" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Distribution Type" dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Minimum" dataDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Maximum" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Mean/Mode" dataDxfId="72"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Standard Deviation" dataDxfId="71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table156" displayName="Table156" ref="A1:M3" totalsRowShown="0" tableBorderDxfId="99">
+  <autoFilter ref="A1:M3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="13">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Internal" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="97"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="96"/>
+    <tableColumn id="10" xr3:uid="{115A314C-6A1B-4509-AD17-EBA48B227F1D}" name="Description" dataDxfId="95"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Units" dataDxfId="94"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Distribution Type" dataDxfId="93"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Minimum" dataDxfId="92"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Maximum" dataDxfId="91"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Mean/Mode" dataDxfId="90"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Standard Deviation" dataDxfId="89"/>
+    <tableColumn id="11" xr3:uid="{1D961365-C163-4709-AB34-FA18998E1C0C}" name="Lower Limit" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{DD91A285-8CA3-48CC-8B2D-6AD307B1829A}" name="Upper Limit" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{289708CC-2479-44B9-8E21-211759607199}" name="Step" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:J4" totalsRowShown="0" tableBorderDxfId="68">
-  <autoFilter ref="A1:J4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Internal" dataDxfId="67"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="65"/>
-    <tableColumn id="10" xr3:uid="{E238511C-0575-407F-83C7-4D6E37CAA1C8}" name="Description" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Units" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Distribution Type" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Minimum" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Maximum" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Mean/Mode" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Standard Deviation" dataDxfId="58"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:M4" totalsRowShown="0" tableBorderDxfId="86">
+  <autoFilter ref="A1:M4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="13">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Internal" dataDxfId="85"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="83"/>
+    <tableColumn id="10" xr3:uid="{E238511C-0575-407F-83C7-4D6E37CAA1C8}" name="Description" dataDxfId="82"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Units" dataDxfId="81"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Distribution Type" dataDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Minimum" dataDxfId="79"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Maximum" dataDxfId="78"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Mean/Mode" dataDxfId="77"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Standard Deviation" dataDxfId="76"/>
+    <tableColumn id="11" xr3:uid="{1D5D06E3-C2FF-4E33-A67E-846C813585DD}" name="Lower Limit" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{59B419A3-4B50-4E25-9295-12F6E479C7C1}" name="Upper Limit" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{B44B2162-0D76-4003-8141-9F91F7CB1D51}" name="Step" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table157" displayName="Table157" ref="A1:J4" totalsRowShown="0" tableBorderDxfId="54">
-  <autoFilter ref="A1:J4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Internal" dataDxfId="53"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Category" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="51"/>
-    <tableColumn id="10" xr3:uid="{82317EA3-EFA1-4204-866F-27AD4E7F4565}" name="Description" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Distribution Type" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Minimum" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Maximum" dataDxfId="46"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Mean/Mode" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Standard Deviation" dataDxfId="44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table157" displayName="Table157" ref="A1:M4" totalsRowShown="0" tableBorderDxfId="72">
+  <autoFilter ref="A1:M4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="13">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Internal" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Category" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="69"/>
+    <tableColumn id="10" xr3:uid="{82317EA3-EFA1-4204-866F-27AD4E7F4565}" name="Description" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Distribution Type" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Minimum" dataDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Maximum" dataDxfId="64"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Mean/Mode" dataDxfId="63"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Standard Deviation" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{D8432F00-68F0-499E-8310-7BEAF2D5BFFA}" name="Lower Limit" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{BCED7806-F146-4B52-AF53-D5DE4EBA4D11}" name="Upper Limit" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{A3158C91-CCDA-42BB-98F8-B1415C87FD9F}" name="Step" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1579" displayName="Table1579" ref="A1:J6" totalsRowShown="0" headerRowBorderDxfId="39" tableBorderDxfId="38">
-  <autoFilter ref="A1:J6" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Internal" dataDxfId="37"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Category" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{832C45C5-9E76-4B8A-83B0-2EB32C68E2FD}" name="Description" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Units" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Distribution Type" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Minimum" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Maximum" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Mean/Mode" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Standard Deviation" dataDxfId="28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1579" displayName="Table1579" ref="A1:M6" totalsRowShown="0" headerRowBorderDxfId="57" tableBorderDxfId="56">
+  <autoFilter ref="A1:M6" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="13">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Internal" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Category" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{832C45C5-9E76-4B8A-83B0-2EB32C68E2FD}" name="Description" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Units" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Distribution Type" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Minimum" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Maximum" dataDxfId="48"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Mean/Mode" dataDxfId="47"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Standard Deviation" dataDxfId="46"/>
+    <tableColumn id="11" xr3:uid="{DB8C4311-5A85-4D8D-A5C2-F47C77E8643D}" name="Lower Limit" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{96A08B49-5A79-4F13-BC86-FC5E2B426E49}" name="Upper Limit" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{D4252238-C1B7-4D7A-B8C5-A52164228F94}" name="Step" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table15793" displayName="Table15793" ref="A1:J2" totalsRowShown="0" headerRowBorderDxfId="25" tableBorderDxfId="24">
-  <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="10">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Internal" dataDxfId="23"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Category" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Name" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{68CD65C3-6212-4FBA-A45A-955FEEA37D44}" name="Description" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Units" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Distribution Type" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Minimum" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Maximum" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Mean/Mode" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Standard Deviation" dataDxfId="14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table15793" displayName="Table15793" ref="A1:M2" insertRow="1" totalsRowShown="0" headerRowBorderDxfId="43" tableBorderDxfId="42">
+  <autoFilter ref="A1:M2" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="13">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Internal" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Category" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Name" dataDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{68CD65C3-6212-4FBA-A45A-955FEEA37D44}" name="Description" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Units" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Distribution Type" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Minimum" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Maximum" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Mean/Mode" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Standard Deviation" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{95D767C7-80C3-48E6-8676-E360CD889508}" name="Lower Limit" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{9CA92EEE-1C69-4662-9FC6-F69DA0AE3671}" name="Upper Limit" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{6140CBF1-6BD2-40E0-9B39-5EA769B73A3B}" name="Step" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157910" displayName="Table157910" ref="A1:J2" totalsRowShown="0" headerRowBorderDxfId="11" tableBorderDxfId="10">
-  <autoFilter ref="A1:J2" xr:uid="{C58E5582-2A25-434F-8C6A-2EF9AC741C58}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157910" displayName="Table157910" ref="A1:M2" totalsRowShown="0" headerRowBorderDxfId="29" tableBorderDxfId="28">
+  <autoFilter ref="A1:M2" xr:uid="{C58E5582-2A25-434F-8C6A-2EF9AC741C58}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J2">
     <sortCondition ref="B1:B2"/>
   </sortState>
-  <tableColumns count="10">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Internal" dataDxfId="9"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Category" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Name" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{63BA373B-667A-4A36-BB6C-997B9631910B}" name="Description" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Units" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Distribution Type" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Minimum" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Maximum" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Mean/Mode" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Standard Deviation" dataDxfId="0"/>
+  <tableColumns count="13">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Internal" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Category" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Name" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{63BA373B-667A-4A36-BB6C-997B9631910B}" name="Description" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Units" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Distribution Type" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Minimum" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Maximum" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Mean/Mode" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Standard Deviation" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{B286B466-1F40-4449-900C-61ACE92313F0}" name="Lower Limit" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{4CAE3350-4ABC-40B6-B059-3A8198700CE1}" name="Upper Limit" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{BC38CFEA-8053-4CB7-B237-C848302F26B7}" name="Step" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2689,10 +3106,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2709,7 +3126,7 @@
     <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -2740,8 +3157,17 @@
       <c r="J1" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>42</v>
@@ -2762,8 +3188,17 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="13" t="s">
         <v>43</v>
@@ -2784,13 +3219,22 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="15"/>
+      <c r="K3" s="14">
+        <v>0</v>
+      </c>
+      <c r="L3" s="14">
+        <v>10</v>
+      </c>
+      <c r="M3" s="14">
+        <v>0.1</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:J3">
-    <cfRule type="expression" dxfId="83" priority="33">
+    <cfRule type="expression" dxfId="101" priority="33">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="34">
+    <cfRule type="expression" dxfId="100" priority="34">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2810,10 +3254,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2830,7 +3274,7 @@
     <col min="10" max="11" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -2861,8 +3305,17 @@
       <c r="J1" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>43</v>
@@ -2883,8 +3336,17 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>20</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>52</v>
@@ -2905,8 +3367,17 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" s="11">
+        <v>0</v>
+      </c>
+      <c r="L3" s="11">
+        <v>20</v>
+      </c>
+      <c r="M3" s="11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>43</v>
@@ -2927,15 +3398,24 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="12"/>
+      <c r="K4" s="14">
+        <v>0</v>
+      </c>
+      <c r="L4" s="14">
+        <v>48</v>
+      </c>
+      <c r="M4" s="14">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:J4">
-    <cfRule type="expression" dxfId="70" priority="17">
+    <cfRule type="expression" dxfId="88" priority="17">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:J4">
-    <cfRule type="expression" dxfId="69" priority="34">
+    <cfRule type="expression" dxfId="87" priority="34">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2954,10 +3434,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2974,7 +3454,7 @@
     <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -3005,8 +3485,17 @@
       <c r="J1" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>42</v>
@@ -3027,8 +3516,17 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>57</v>
@@ -3049,8 +3547,17 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" s="11">
+        <v>0</v>
+      </c>
+      <c r="L3" s="11">
+        <v>10000</v>
+      </c>
+      <c r="M3" s="11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>52</v>
@@ -3071,20 +3578,29 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="12"/>
+      <c r="K4" s="14">
+        <v>0</v>
+      </c>
+      <c r="L4" s="14">
+        <v>10</v>
+      </c>
+      <c r="M4" s="14">
+        <v>0.1</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:J4">
-    <cfRule type="expression" dxfId="57" priority="19">
+    <cfRule type="expression" dxfId="75" priority="19">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:J3 A4:C4 E4:J4">
-    <cfRule type="expression" dxfId="56" priority="32">
+    <cfRule type="expression" dxfId="74" priority="32">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="55" priority="1">
+    <cfRule type="expression" dxfId="73" priority="1">
       <formula>ISBLANK($F4)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3103,10 +3619,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3123,7 +3639,7 @@
     <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -3154,8 +3670,17 @@
       <c r="J1" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>42</v>
@@ -3176,8 +3701,17 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="11" t="s">
         <v>43</v>
@@ -3198,8 +3732,17 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="12"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" s="11">
+        <v>100</v>
+      </c>
+      <c r="L3" s="11">
+        <v>2000</v>
+      </c>
+      <c r="M3" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
         <v>43</v>
@@ -3220,8 +3763,17 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="12"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" s="11">
+        <v>100</v>
+      </c>
+      <c r="L4" s="11">
+        <v>2000</v>
+      </c>
+      <c r="M4" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
         <v>43</v>
@@ -3242,8 +3794,17 @@
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5" s="11">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11">
+        <v>1</v>
+      </c>
+      <c r="M5" s="11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
         <v>52</v>
@@ -3264,25 +3825,34 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="12"/>
+      <c r="K6" s="14">
+        <v>0</v>
+      </c>
+      <c r="L6" s="14">
+        <v>10</v>
+      </c>
+      <c r="M6" s="14">
+        <v>0.1</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:J6">
-    <cfRule type="expression" dxfId="43" priority="23">
+    <cfRule type="expression" dxfId="61" priority="23">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:J5 A2:C2 E2:J2 A6:C6 E6:J6">
-    <cfRule type="expression" dxfId="42" priority="32">
+    <cfRule type="expression" dxfId="60" priority="32">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="41" priority="2">
+    <cfRule type="expression" dxfId="59" priority="2">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="40" priority="1">
+    <cfRule type="expression" dxfId="58" priority="1">
       <formula>ISBLANK($F6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3300,10 +3870,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K1" sqref="K1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3320,7 +3890,7 @@
     <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -3351,8 +3921,17 @@
       <c r="J1" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3363,15 +3942,18 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="4"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:J2">
-    <cfRule type="expression" dxfId="27" priority="24">
+    <cfRule type="expression" dxfId="45" priority="24">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:J2">
-    <cfRule type="expression" dxfId="26" priority="29">
+    <cfRule type="expression" dxfId="44" priority="29">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3390,10 +3972,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3410,7 +3992,7 @@
     <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -3441,8 +4023,17 @@
       <c r="J1" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>43</v>
@@ -3463,15 +4054,24 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="4"/>
+      <c r="K2" s="16">
+        <v>20</v>
+      </c>
+      <c r="L2" s="16">
+        <v>500</v>
+      </c>
+      <c r="M2" s="16">
+        <v>0.1</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:J2">
-    <cfRule type="expression" dxfId="13" priority="27">
+    <cfRule type="expression" dxfId="31" priority="27">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:J2">
-    <cfRule type="expression" dxfId="12" priority="28">
+    <cfRule type="expression" dxfId="30" priority="28">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>